<commit_message>
working with linux HID
</commit_message>
<xml_diff>
--- a/data/2019.xlsx
+++ b/data/2019.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="5" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="989" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="01 - January" sheetId="1" state="visible" r:id="rId1"/>
@@ -21,20 +21,35 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="12 - December" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -54,16 +69,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+  <cellStyles count="6">
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" name="Comma" xfId="1"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
+    <cellStyle builtinId="4" name="Currency" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="5" name="Percent" xfId="5"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -352,216 +384,738 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <cols>
+    <col customWidth="1" max="1025" min="1" style="1" width="8.570850202429151"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15" r="1" s="2">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <cols>
+    <col customWidth="1" max="1025" min="1" style="1" width="8.570850202429151"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15" r="1" s="2">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <cols>
+    <col customWidth="1" max="1025" min="1" style="1" width="8.570850202429151"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15" r="1" s="2">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <cols>
+    <col customWidth="1" max="1025" min="1" style="1" width="8.570850202429151"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15" r="1" s="2">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <cols>
+    <col customWidth="1" max="1025" min="1" style="1" width="8.570850202429151"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15" r="1" s="2">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <cols>
+    <col customWidth="1" max="1025" min="1" style="1" width="8.570850202429151"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15" r="1" s="2">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <cols>
+    <col customWidth="1" max="1025" min="1" style="1" width="8.570850202429151"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15" r="1" s="2">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <cols>
+    <col customWidth="1" max="1025" min="1" style="1" width="8.570850202429151"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15" r="1" s="2">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" style="1" width="14.1093117408907"/>
+    <col customWidth="1" max="2" min="2" style="1" width="20.6153846153846"/>
+    <col customWidth="1" max="1025" min="3" style="1" width="8.570850202429151"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15" r="1" s="2">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="2" s="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>09 - Sunday</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>0016581666</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>22:53:55</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>22:54:03</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>22:54:07</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>22:54:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>10 - Monday</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>0016581666</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>00:18:11</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>00:18:15</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>00:27:00</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="inlineStr">
+        <is>
+          <t>00:28:22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <cols>
+    <col customWidth="1" max="1025" min="1" style="1" width="8.570850202429151"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15" r="1" s="2">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <cols>
+    <col customWidth="1" max="1025" min="1" style="1" width="8.570850202429151"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15" r="1" s="2">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <cols>
+    <col customWidth="1" max="1025" min="1" style="1" width="8.570850202429151"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15" r="1" s="2">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>